<commit_message>
Implemented grid search, added transfer learning architectures
Added a function to grid search hyper-parameters.

Added 4 more transfer learning architectures (InceptionResNetV2, MobileNetV2, DenseNet201, Xception)

Added Binta ResNet50 Type 1 architecture to test on my dataset.
</commit_message>
<xml_diff>
--- a/Model Training Results.xlsx
+++ b/Model Training Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiyrahkeith/Documents/GitHub/Face Identification - CZoo/FaceIdentification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5940C06D-5EB8-6A4C-800B-BF705C460260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5612C3-8A45-D043-8D26-A57D06170E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="680" windowWidth="34580" windowHeight="17440" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
+    <workbookView xWindow="2320" yWindow="2480" windowWidth="34580" windowHeight="17440" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="6">
+  <futureMetadata name="XLRICHVALUE" count="7">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -83,8 +83,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="6">
+  <valueMetadata count="7">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -103,12 +110,15 @@
     <bk>
       <rc t="1" v="5"/>
     </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="57">
   <si>
     <t>Model Name</t>
   </si>
@@ -182,9 +192,6 @@
     <t>Due to Binta_VGG16_Type 1 converging so quickly to a low accuracy, I wanted to see if the second proposed architecture would follow a similar loss &amp; accuracy curve. I confirmed that it did.</t>
   </si>
   <si>
-    <t>VGG16_Default</t>
-  </si>
-  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -237,6 +244,51 @@
   </si>
   <si>
     <t>The overall accuracy was decreased by ~8% from the un-augmented version, but the validation accuracy showed a substantial increase of ~30%, meaning that the image augmentation really helped with overfitting.</t>
+  </si>
+  <si>
+    <t>Binta_ResNet50_Type 1</t>
+  </si>
+  <si>
+    <t>(Decay) learning rate / epochs</t>
+  </si>
+  <si>
+    <t>VGG-16_Default</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2</t>
+  </si>
+  <si>
+    <t>MobileNetV2</t>
+  </si>
+  <si>
+    <t>DenseNet201</t>
+  </si>
+  <si>
+    <t>Xception</t>
+  </si>
+  <si>
+    <t>75s/epoch</t>
+  </si>
+  <si>
+    <t>71s/epoch</t>
+  </si>
+  <si>
+    <t>19s/epoch</t>
+  </si>
+  <si>
+    <t>127s/epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32s/epoch. Best accuracy of all the models by over 15%. It did not overfit, the validation accuracy was 5% better than the training accuracy. </t>
+  </si>
+  <si>
+    <t>82s/epoch. Second best accuracy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46s/epoch. Third best accuracy. </t>
   </si>
 </sst>
 </file>
@@ -259,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +342,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -303,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,6 +412,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -414,7 +487,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -439,6 +512,10 @@
     <v>5</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -459,6 +536,7 @@
   <rel r:id="rId4"/>
   <rel r:id="rId5"/>
   <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
 </richValueRels>
 </file>
 
@@ -779,11 +857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF77D116-1000-2A40-9EE0-79918EBDE034}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,12 +875,12 @@
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="2" customWidth="1"/>
     <col min="11" max="11" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61" style="2" customWidth="1"/>
+    <col min="15" max="15" width="92" style="2" customWidth="1"/>
     <col min="16" max="16" width="35.33203125" style="2" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -835,7 +913,7 @@
       <c r="I1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="16" t="s">
@@ -883,7 +961,7 @@
       <c r="I2" s="5">
         <v>1E-4</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="6">
         <v>0.9</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -931,7 +1009,7 @@
       <c r="I3" s="5">
         <v>1E-4</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="6">
         <v>0.9</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -956,7 +1034,7 @@
         <v>45516</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4">
         <v>0.05</v>
@@ -979,7 +1057,7 @@
       <c r="I4" s="5">
         <v>1E-4</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="6">
         <v>0.9</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -995,73 +1073,71 @@
         <v>19</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>45514</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>45517</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4">
+        <v>7.2099999999999997E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4">
+        <v>100</v>
+      </c>
+      <c r="G5" s="4">
+        <v>32</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.16</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8">
-        <v>10</v>
-      </c>
-      <c r="G5" s="8">
-        <v>32</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="8" t="s">
+      <c r="I5" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="4">
         <v>0.1</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="10" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P5" s="11"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>45514</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C6" s="8">
-        <v>0.317</v>
+        <v>0.19</v>
       </c>
       <c r="D6" s="8">
-        <v>0.30399999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F6" s="8">
         <v>10</v>
@@ -1070,13 +1146,13 @@
         <v>32</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="9">
         <v>1E-3</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>26</v>
+      <c r="J6" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>11</v>
@@ -1090,26 +1166,26 @@
       <c r="N6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="10" t="e" vm="2">
+      <c r="O6" s="10" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>45514</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.317</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.41</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="F7" s="8">
         <v>10</v>
@@ -1118,13 +1194,13 @@
         <v>32</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="9">
         <v>1E-3</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>26</v>
+      <c r="J7" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>11</v>
@@ -1138,72 +1214,72 @@
       <c r="N7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="10"/>
+      <c r="O7" s="10" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
-        <v>45516</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.77729999999999999</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13">
-        <v>60</v>
-      </c>
-      <c r="G8" s="13">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>45514</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="8">
         <v>32</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="8">
         <v>0.1</v>
       </c>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="15" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P8" s="15"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>45516</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="13">
-        <v>0.64839999999999998</v>
+        <v>0.77729999999999999</v>
       </c>
       <c r="D9" s="13">
-        <v>0.45839999999999997</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="13">
         <v>60</v>
@@ -1212,13 +1288,13 @@
         <v>32</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="14">
         <v>1E-3</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>26</v>
+      <c r="J9" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>11</v>
@@ -1230,30 +1306,28 @@
         <v>0.1</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="15" t="e" vm="4">
+        <v>19</v>
+      </c>
+      <c r="O9" s="15" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="P9" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="P9" s="15"/>
     </row>
     <row r="10" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>45516</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C10" s="13">
-        <v>0.56510000000000005</v>
+        <v>0.64839999999999998</v>
       </c>
       <c r="D10" s="13">
-        <v>0.47310000000000002</v>
+        <v>0.45839999999999997</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="13">
         <v>60</v>
@@ -1262,13 +1336,13 @@
         <v>32</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="14">
         <v>1E-3</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>26</v>
+      <c r="J10" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>11</v>
@@ -1280,13 +1354,13 @@
         <v>0.1</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="15" t="e" vm="5">
+        <v>33</v>
+      </c>
+      <c r="O10" s="15" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
@@ -1294,16 +1368,16 @@
         <v>45516</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" s="13">
-        <v>0.69110000000000005</v>
+        <v>0.56510000000000005</v>
       </c>
       <c r="D11" s="13">
-        <v>0.71379999999999999</v>
+        <v>0.47310000000000002</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="13">
         <v>60</v>
@@ -1312,13 +1386,13 @@
         <v>32</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="14">
         <v>1E-3</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>26</v>
+      <c r="J11" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>11</v>
@@ -1330,16 +1404,407 @@
         <v>0.1</v>
       </c>
       <c r="N11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="15" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>45516</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.71379999999999999</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="13">
+        <v>60</v>
+      </c>
+      <c r="G12" s="13">
+        <v>32</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="15" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="15" t="e" vm="6">
+    </row>
+    <row r="13" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0.22159999999999999</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.2442</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="20">
+        <v>30</v>
+      </c>
+      <c r="G13" s="20">
+        <v>32</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="21">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="22" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="15" t="s">
-        <v>42</v>
+      <c r="P13" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.44990000000000002</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.50429999999999997</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="20">
+        <v>30</v>
+      </c>
+      <c r="G14" s="20">
+        <v>32</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="21">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="20">
+        <v>2.1</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="22"/>
+      <c r="P14" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0.65590000000000004</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="20">
+        <v>30</v>
+      </c>
+      <c r="G15" s="20">
+        <v>32</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="21">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="22"/>
+      <c r="P15" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="20">
+        <v>0.4032</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.41889999999999999</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="20">
+        <v>30</v>
+      </c>
+      <c r="G16" s="20">
+        <v>32</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="21">
+        <v>4.0010000000000003</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0.43809999999999999</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.46949999999999997</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="20">
+        <v>30</v>
+      </c>
+      <c r="G17" s="20">
+        <v>32</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="21">
+        <v>5.0010000000000003</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0.49809999999999999</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="20">
+        <v>30</v>
+      </c>
+      <c r="G18" s="20">
+        <v>32</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="21">
+        <v>6.0010000000000003</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="20">
+        <v>6.1</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>45517</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0.4259</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.4703</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="20">
+        <v>30</v>
+      </c>
+      <c r="G19" s="20">
+        <v>32</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="21">
+        <v>7.0010000000000003</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="20">
+        <v>7.1</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O13:O15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed dataset statistics bug
Fixed a bug in Dataset_Statistics.py that undercounted the number of individuals in a dataset.

Updated the other scripts to test a new set of hyper-parameters for the grid search.
</commit_message>
<xml_diff>
--- a/Model Training Results.xlsx
+++ b/Model Training Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiyrahkeith/Documents/GitHub/Face Identification - CZoo/FaceIdentification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5612C3-8A45-D043-8D26-A57D06170E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F874A0-58BB-854A-86E2-3FC61599B8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="2480" windowWidth="34580" windowHeight="17440" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
+    <workbookView xWindow="2200" yWindow="780" windowWidth="34580" windowHeight="17440" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="57">
   <si>
     <t>Model Name</t>
   </si>
@@ -270,32 +270,32 @@
     <t>Xception</t>
   </si>
   <si>
-    <t>75s/epoch</t>
-  </si>
-  <si>
-    <t>71s/epoch</t>
-  </si>
-  <si>
-    <t>19s/epoch</t>
-  </si>
-  <si>
-    <t>127s/epoch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32s/epoch. Best accuracy of all the models by over 15%. It did not overfit, the validation accuracy was 5% better than the training accuracy. </t>
-  </si>
-  <si>
-    <t>82s/epoch. Second best accuracy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46s/epoch. Third best accuracy. </t>
+    <t>Time (s/epoch)</t>
+  </si>
+  <si>
+    <t>All models in this green section have the same architecture on top of the transfer learning model as is shown for the purple (_default) models above.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third best accuracy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Best accuracy of all the models by over 15%. It did not overfit, the validation accuracy was 5% better than the training accuracy. </t>
+  </si>
+  <si>
+    <t>Second best accuracy</t>
+  </si>
+  <si>
+    <t>RMSProp</t>
+  </si>
+  <si>
+    <t>1st best accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +306,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -857,11 +863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF77D116-1000-2A40-9EE0-79918EBDE034}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,16 +882,16 @@
     <col min="8" max="8" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="92" style="2" customWidth="1"/>
-    <col min="16" max="16" width="35.33203125" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="28.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="24.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="92" style="2" customWidth="1"/>
+    <col min="17" max="17" width="35.33203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -929,11 +935,14 @@
         <v>20</v>
       </c>
       <c r="O1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="17"/>
-    </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="Q1" s="17"/>
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45514</v>
       </c>
@@ -976,12 +985,15 @@
       <c r="N2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="6">
+        <v>14</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45514</v>
       </c>
@@ -1024,12 +1036,15 @@
       <c r="N3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="6">
+        <v>14</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45516</v>
       </c>
@@ -1072,12 +1087,15 @@
       <c r="N4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="6">
+        <v>24</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45517</v>
       </c>
@@ -1120,10 +1138,13 @@
       <c r="N5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>45514</v>
       </c>
@@ -1166,12 +1187,15 @@
       <c r="N6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="10" t="e" vm="1">
+      <c r="O6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="10" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>45514</v>
       </c>
@@ -1214,12 +1238,15 @@
       <c r="N7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="10" t="e" vm="2">
+      <c r="O7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="10" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>45514</v>
       </c>
@@ -1262,10 +1289,13 @@
       <c r="N8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>45516</v>
       </c>
@@ -1308,12 +1338,15 @@
       <c r="N9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="15" t="e" vm="3">
+      <c r="O9" s="15"/>
+      <c r="P9" s="15" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="P9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q9" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>45516</v>
       </c>
@@ -1356,14 +1389,15 @@
       <c r="N10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="15" t="e" vm="4">
+      <c r="O10" s="15"/>
+      <c r="P10" s="15" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="Q10" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>45516</v>
       </c>
@@ -1406,14 +1440,15 @@
       <c r="N11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="15" t="e" vm="5">
+      <c r="O11" s="15"/>
+      <c r="P11" s="15" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="Q11" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>45516</v>
       </c>
@@ -1456,14 +1491,15 @@
       <c r="N12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="15" t="e" vm="6">
+      <c r="O12" s="15"/>
+      <c r="P12" s="15" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="Q12" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>45517</v>
       </c>
@@ -1501,19 +1537,22 @@
         <v>16</v>
       </c>
       <c r="M13" s="20">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="N13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="22" t="e" vm="7">
+      <c r="O13" s="19">
+        <v>75</v>
+      </c>
+      <c r="P13" s="22" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="P13" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q13" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>45517</v>
       </c>
@@ -1539,7 +1578,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="21">
-        <v>2.0009999999999999</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>25</v>
@@ -1551,17 +1590,20 @@
         <v>16</v>
       </c>
       <c r="M14" s="20">
-        <v>2.1</v>
+        <v>0.1</v>
       </c>
       <c r="N14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O14" s="19">
+        <v>46</v>
+      </c>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>45517</v>
       </c>
@@ -1587,7 +1629,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="21">
-        <v>3.0009999999999999</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>25</v>
@@ -1599,17 +1641,20 @@
         <v>16</v>
       </c>
       <c r="M15" s="20">
-        <v>3.1</v>
+        <v>0.1</v>
       </c>
       <c r="N15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="19">
+        <v>32</v>
+      </c>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>45517</v>
       </c>
@@ -1635,7 +1680,7 @@
         <v>24</v>
       </c>
       <c r="I16" s="21">
-        <v>4.0010000000000003</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>25</v>
@@ -1647,17 +1692,18 @@
         <v>16</v>
       </c>
       <c r="M16" s="20">
-        <v>4.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="N16" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O16" s="19">
+        <v>71</v>
+      </c>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+    </row>
+    <row r="17" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>45517</v>
       </c>
@@ -1683,7 +1729,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="21">
-        <v>5.0010000000000003</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>25</v>
@@ -1695,17 +1741,18 @@
         <v>16</v>
       </c>
       <c r="M17" s="20">
-        <v>5.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="N17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O17" s="19">
+        <v>19</v>
+      </c>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+    </row>
+    <row r="18" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>45517</v>
       </c>
@@ -1731,7 +1778,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="21">
-        <v>6.0010000000000003</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>25</v>
@@ -1743,17 +1790,20 @@
         <v>16</v>
       </c>
       <c r="M18" s="20">
-        <v>6.1</v>
+        <v>0.1</v>
       </c>
       <c r="N18" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O18" s="19">
+        <v>82</v>
+      </c>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>45517</v>
       </c>
@@ -1779,7 +1829,7 @@
         <v>24</v>
       </c>
       <c r="I19" s="21">
-        <v>7.0010000000000003</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>25</v>
@@ -1791,20 +1841,1788 @@
         <v>16</v>
       </c>
       <c r="M19" s="20">
-        <v>7.1</v>
+        <v>0.1</v>
       </c>
       <c r="N19" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="O19" s="19">
+        <v>127</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+    </row>
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.60540000000000005</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.63790000000000002</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4">
+        <v>60</v>
+      </c>
+      <c r="G20" s="4">
+        <v>16</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" s="6">
+        <v>35</v>
+      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.61519999999999997</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.6593</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="4">
+        <v>60</v>
+      </c>
+      <c r="G21" s="4">
+        <v>16</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="6">
+        <v>34</v>
+      </c>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.38159999999999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.4672</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="4">
+        <v>60</v>
+      </c>
+      <c r="G22" s="4">
+        <v>16</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O22" s="6">
+        <v>34</v>
+      </c>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.1389</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="4">
+        <v>60</v>
+      </c>
+      <c r="G23" s="4">
+        <v>16</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O23" s="6">
+        <v>34</v>
+      </c>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.2387</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="4">
+        <v>60</v>
+      </c>
+      <c r="G24" s="4">
+        <v>16</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O24" s="6">
+        <v>34</v>
+      </c>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.62519999999999998</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.65449999999999997</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="4">
+        <v>60</v>
+      </c>
+      <c r="G25" s="4">
+        <v>16</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O25" s="6">
+        <v>34</v>
+      </c>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.68820000000000003</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="4">
+        <v>60</v>
+      </c>
+      <c r="G26" s="4">
+        <v>16</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O26" s="6">
+        <v>34</v>
+      </c>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.71860000000000002</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.75729999999999997</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="4">
+        <v>60</v>
+      </c>
+      <c r="G27" s="4">
+        <v>16</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O27" s="6">
+        <v>35</v>
+      </c>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.2681</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.18890000000000001</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="4">
+        <v>60</v>
+      </c>
+      <c r="G28" s="4">
+        <v>16</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O28" s="6">
+        <v>36</v>
+      </c>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.57069999999999999</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.60550000000000004</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="4">
+        <v>60</v>
+      </c>
+      <c r="G29" s="4">
+        <v>16</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O29" s="6">
+        <v>36</v>
+      </c>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.69620000000000004</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.72960000000000003</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="4">
+        <v>60</v>
+      </c>
+      <c r="G30" s="4">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O30" s="6">
+        <v>36</v>
+      </c>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.71489999999999998</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.74150000000000005</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="4">
+        <v>60</v>
+      </c>
+      <c r="G31" s="4">
+        <v>16</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" s="6">
+        <v>36</v>
+      </c>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.5867</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="4">
+        <v>60</v>
+      </c>
+      <c r="G32" s="4">
+        <v>16</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O32" s="6">
+        <v>31</v>
+      </c>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+    </row>
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.5806</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.6482</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="4">
+        <v>60</v>
+      </c>
+      <c r="G33" s="4">
+        <v>32</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" s="6">
+        <v>31</v>
+      </c>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+    </row>
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.3755</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="4">
+        <v>60</v>
+      </c>
+      <c r="G34" s="4">
+        <v>32</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O34" s="6">
+        <v>31</v>
+      </c>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.10390000000000001</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="4">
+        <v>60</v>
+      </c>
+      <c r="G35" s="4">
+        <v>32</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O35" s="6">
+        <v>32</v>
+      </c>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.34029999999999999</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.35970000000000002</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="4">
+        <v>60</v>
+      </c>
+      <c r="G36" s="4">
+        <v>32</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J36" s="6">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O36" s="6">
+        <v>32</v>
+      </c>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.59470000000000001</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.6008</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="4">
+        <v>60</v>
+      </c>
+      <c r="G37" s="4">
+        <v>32</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O37" s="6">
+        <v>32</v>
+      </c>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.72719999999999996</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="4">
+        <v>60</v>
+      </c>
+      <c r="G38" s="4">
+        <v>32</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J38" s="6">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O38" s="6">
+        <v>32</v>
+      </c>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.69879999999999998</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="4">
+        <v>60</v>
+      </c>
+      <c r="G39" s="4">
+        <v>32</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J39" s="6">
+        <v>0</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O39" s="6">
+        <v>32</v>
+      </c>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.24410000000000001</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.25140000000000001</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="4">
+        <v>60</v>
+      </c>
+      <c r="G40" s="4">
+        <v>32</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J40" s="6">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O40" s="6">
+        <v>32</v>
+      </c>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.57379999999999998</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.59760000000000002</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="4">
+        <v>60</v>
+      </c>
+      <c r="G41" s="4">
+        <v>32</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J41" s="6">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O41" s="6">
+        <v>32</v>
+      </c>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.67610000000000003</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.71689999999999998</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="4">
+        <v>60</v>
+      </c>
+      <c r="G42" s="4">
+        <v>32</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J42" s="6">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" s="6">
+        <v>32</v>
+      </c>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="4">
+        <v>60</v>
+      </c>
+      <c r="G43" s="4">
+        <v>32</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J43" s="6">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O43" s="6">
+        <v>32</v>
+      </c>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+    </row>
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.62470000000000003</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.66479999999999995</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="4">
+        <v>60</v>
+      </c>
+      <c r="G44" s="4">
+        <v>64</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J44" s="6">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O44" s="6">
+        <v>30</v>
+      </c>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+    </row>
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.51270000000000004</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.5897</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="4">
+        <v>60</v>
+      </c>
+      <c r="G45" s="4">
+        <v>64</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J45" s="6">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O45" s="6">
+        <v>30</v>
+      </c>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.2369</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.29559999999999997</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="4">
+        <v>60</v>
+      </c>
+      <c r="G46" s="4">
+        <v>64</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J46" s="6">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O46" s="6">
+        <v>31</v>
+      </c>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="4">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="D47" s="4">
+        <v>9.7199999999999995E-2</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="4">
+        <v>60</v>
+      </c>
+      <c r="G47" s="4">
+        <v>64</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J47" s="6">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O47" s="6">
+        <v>31</v>
+      </c>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.3473</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.36130000000000001</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="4">
+        <v>60</v>
+      </c>
+      <c r="G48" s="4">
+        <v>64</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J48" s="6">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O48" s="6">
+        <v>31</v>
+      </c>
+      <c r="P48" s="6"/>
+      <c r="Q48" s="6"/>
+    </row>
+    <row r="49" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.52790000000000004</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="4">
+        <v>60</v>
+      </c>
+      <c r="G49" s="4">
+        <v>64</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J49" s="6">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O49" s="6">
+        <v>31</v>
+      </c>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+    </row>
+    <row r="50" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0.72250000000000003</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="4">
+        <v>60</v>
+      </c>
+      <c r="G50" s="4">
+        <v>64</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J50" s="6">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M50" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O50" s="6">
+        <v>31</v>
+      </c>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+    </row>
+    <row r="51" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.70430000000000004</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="4">
+        <v>60</v>
+      </c>
+      <c r="G51" s="4">
+        <v>64</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J51" s="6">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O51" s="6">
+        <v>31</v>
+      </c>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+    </row>
+    <row r="52" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.24390000000000001</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0.20080000000000001</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="4">
+        <v>60</v>
+      </c>
+      <c r="G52" s="4">
+        <v>64</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J52" s="6">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M52" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O52" s="6">
+        <v>31</v>
+      </c>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+    </row>
+    <row r="53" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.5333</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0.55489999999999995</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="4">
+        <v>60</v>
+      </c>
+      <c r="G53" s="4">
+        <v>64</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J53" s="6">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O53" s="6">
+        <v>31</v>
+      </c>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.69130000000000003</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.71779999999999999</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="4">
+        <v>60</v>
+      </c>
+      <c r="G54" s="4">
+        <v>64</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J54" s="6">
+        <v>0</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M54" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O54" s="6">
+        <v>31</v>
+      </c>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="6"/>
+    </row>
+    <row r="55" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>45519</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.66610000000000003</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0.71940000000000004</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="4">
+        <v>60</v>
+      </c>
+      <c r="G55" s="4">
+        <v>64</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J55" s="6">
+        <v>0</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M55" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O55" s="6">
+        <v>31</v>
+      </c>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O13:O15"/>
+    <mergeCell ref="P13:P15"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Training search for top layers
Added model training to try multiple architectures of layers on top of the transfer learning model.
</commit_message>
<xml_diff>
--- a/Model Training Results.xlsx
+++ b/Model Training Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiyrahkeith/Documents/GitHub/Face Identification - CZoo/FaceIdentification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F874A0-58BB-854A-86E2-3FC61599B8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A86F7FF-4662-134A-BE9A-62A31729EEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="780" windowWidth="34580" windowHeight="17440" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{493026E3-7BC6-834B-B0B6-6CE84E68F60D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="7">
+  <futureMetadata name="XLRICHVALUE" count="21">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -90,8 +90,106 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="7">
+  <valueMetadata count="21">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -113,12 +211,54 @@
     <bk>
       <rc t="1" v="6"/>
     </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="83">
   <si>
     <t>Model Name</t>
   </si>
@@ -249,9 +389,6 @@
     <t>Binta_ResNet50_Type 1</t>
   </si>
   <si>
-    <t>(Decay) learning rate / epochs</t>
-  </si>
-  <si>
     <t>VGG-16_Default</t>
   </si>
   <si>
@@ -289,6 +426,87 @@
   </si>
   <si>
     <t>1st best accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All high results had a learning rate of 0.001 or 0.0001. All high results had optimizer of Adam or RMSProp, but this did not factor in momentum, so SGD could potentially result in higher results if momentum was used. Batch size does not appear to affect results. Overall, validation accuracy was higher than training accuracy.  </t>
+  </si>
+  <si>
+    <t>This blue section represents a grid seach of hyperparameters. It varies the optimizer between Adam, SGD, and RMSProp (with no momentum or decay). It varies learning rate from 0.1, 0.01, 0.001, and 0.0001. And it varies batch size from 16, 32, and 64.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surprisingly, among the SGD results, the ones with larger learning rates (0.1 and 0.01) significantly outperformed the ones with smaller learning rates (0.001 and 0.0001). And although the SGD runs didn't get above the 0.7 accuracy threshold for top results, the top SGD result (with 0.1 LR) did get to 0.66, which is ~5% away from the rest of the top results.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All models were trained with the default architecture layers on top of the transfer training as is shown in the purple section above. </t>
+  </si>
+  <si>
+    <t>SGD_No Momentum</t>
+  </si>
+  <si>
+    <t>SGD_Momentum</t>
+  </si>
+  <si>
+    <t>RMSProp_No Momentum</t>
+  </si>
+  <si>
+    <t>RMSProp_Momentum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For SGD, adding momentum significantly increased accuracy. Whereas, the opposite effective happened with RMSProp, and having 0.0 momentum performed better than 0.9. </t>
+  </si>
+  <si>
+    <t>Generalization_AFD</t>
+  </si>
+  <si>
+    <t>AFD</t>
+  </si>
+  <si>
+    <t>I used the same hyper-parameters as was the best accuracy in the blue grid search of hyper-parameters above. I wanted to see if the individual identification results from Czoo would generalize well to a more course-grained species identification from the AFD dataset. The training did better than expected and converged quickly to a high accuracy in a minimal number of epochs. And this was even with no data augmentations.</t>
+  </si>
+  <si>
+    <t>Generalization_Ctai</t>
+  </si>
+  <si>
+    <t>Ctai</t>
+  </si>
+  <si>
+    <t>Top0</t>
+  </si>
+  <si>
+    <t>Top1</t>
+  </si>
+  <si>
+    <t>Top2</t>
+  </si>
+  <si>
+    <t>Top3</t>
+  </si>
+  <si>
+    <t>Top4</t>
+  </si>
+  <si>
+    <t>Top5</t>
+  </si>
+  <si>
+    <t>Top6</t>
+  </si>
+  <si>
+    <t>Top7</t>
+  </si>
+  <si>
+    <t>Decay = learning rate / epochs</t>
+  </si>
+  <si>
+    <t>The validation accuracy was ~6% less than the top score, but the curve was a lot less erratic during training.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st best training accuracy. Overfitting by ~17%, but its validation accuracy is still higher than even the training accuracy of the other architectures. </t>
+  </si>
+  <si>
+    <t>All of the models showed rapidly fluxuating validation accuracy during training.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top2 did not achieve the top accuracy (~6% lower than Top0), but it had higher validation accuracy. Additionally, it converged very quickly and reached almost top accuracy in 15-20 epochs. Its validation accuracy also showed a much less erratic curve than Top1. </t>
   </si>
 </sst>
 </file>
@@ -317,7 +535,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +572,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BE9E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -367,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,7 +656,34 @@
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,6 +692,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8BE9E7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -493,7 +749,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="21">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -522,6 +778,62 @@
     <v>6</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -543,6 +855,20 @@
   <rel r:id="rId5"/>
   <rel r:id="rId6"/>
   <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
 </richValueRels>
 </file>
 
@@ -863,11 +1189,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF77D116-1000-2A40-9EE0-79918EBDE034}">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,11 +1213,13 @@
     <col min="13" max="13" width="14.83203125" style="1" customWidth="1"/>
     <col min="14" max="15" width="24.6640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="92" style="2" customWidth="1"/>
-    <col min="17" max="17" width="35.33203125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="51.83203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="46.83203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="68.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -935,14 +1263,15 @@
         <v>20</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>18</v>
       </c>
       <c r="Q1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45514</v>
       </c>
@@ -992,8 +1321,9 @@
         <v>21</v>
       </c>
       <c r="Q2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45514</v>
       </c>
@@ -1043,8 +1373,9 @@
         <v>23</v>
       </c>
       <c r="Q3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45516</v>
       </c>
@@ -1094,8 +1425,9 @@
         <v>31</v>
       </c>
       <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45517</v>
       </c>
@@ -1124,7 +1456,7 @@
         <v>1E-4</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>11</v>
@@ -1143,13 +1475,14 @@
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" s="8" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>45514</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="8">
         <v>0.19</v>
@@ -1194,8 +1527,9 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q6" s="11"/>
-    </row>
-    <row r="7" spans="1:17" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R6" s="11"/>
+    </row>
+    <row r="7" spans="1:18" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>45514</v>
       </c>
@@ -1245,8 +1579,9 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q7" s="11"/>
-    </row>
-    <row r="8" spans="1:17" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>45514</v>
       </c>
@@ -1294,8 +1629,9 @@
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:18" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>45516</v>
       </c>
@@ -1345,8 +1681,9 @@
       <c r="Q9" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>45516</v>
       </c>
@@ -1396,8 +1733,9 @@
       <c r="Q10" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R10" s="15"/>
+    </row>
+    <row r="11" spans="1:18" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>45516</v>
       </c>
@@ -1447,8 +1785,9 @@
       <c r="Q11" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" s="13" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>45516</v>
       </c>
@@ -1498,8 +1837,9 @@
       <c r="Q12" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>45517</v>
       </c>
@@ -1545,19 +1885,20 @@
       <c r="O13" s="19">
         <v>75</v>
       </c>
-      <c r="P13" s="22" t="e" vm="7">
+      <c r="P13" s="25" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="R13" s="19"/>
+    </row>
+    <row r="14" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>45517</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="20">
         <v>0.44990000000000002</v>
@@ -1598,12 +1939,13 @@
       <c r="O14" s="19">
         <v>46</v>
       </c>
-      <c r="P14" s="22"/>
+      <c r="P14" s="25"/>
       <c r="Q14" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R14" s="19"/>
+    </row>
+    <row r="15" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>45517</v>
       </c>
@@ -1649,17 +1991,18 @@
       <c r="O15" s="19">
         <v>32</v>
       </c>
-      <c r="P15" s="22"/>
+      <c r="P15" s="25"/>
       <c r="Q15" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="R15" s="19"/>
+    </row>
+    <row r="16" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>45517</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="20">
         <v>0.4032</v>
@@ -1668,7 +2011,7 @@
         <v>0.41889999999999999</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="20">
         <v>30</v>
@@ -1702,13 +2045,14 @@
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
-    </row>
-    <row r="17" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R16" s="19"/>
+    </row>
+    <row r="17" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>45517</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="20">
         <v>0.43809999999999999</v>
@@ -1717,7 +2061,7 @@
         <v>0.46949999999999997</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="20">
         <v>30</v>
@@ -1751,13 +2095,14 @@
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
-    </row>
-    <row r="18" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R17" s="19"/>
+    </row>
+    <row r="18" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>45517</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="20">
         <v>0.49809999999999999</v>
@@ -1766,7 +2111,7 @@
         <v>0.55249999999999999</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="20">
         <v>30</v>
@@ -1800,15 +2145,16 @@
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="R18" s="19"/>
+    </row>
+    <row r="19" spans="1:18" s="20" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>45517</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="20">
         <v>0.4259</v>
@@ -1817,7 +2163,7 @@
         <v>0.4703</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="20">
         <v>30</v>
@@ -1851,8 +2197,9 @@
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
-    </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R19" s="19"/>
+    </row>
+    <row r="20" spans="1:18" s="4" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>45519</v>
       </c>
@@ -1898,10 +2245,15 @@
       <c r="O20" s="6">
         <v>35</v>
       </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="P20" s="26" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>45519</v>
       </c>
@@ -1947,10 +2299,13 @@
       <c r="O21" s="6">
         <v>34</v>
       </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="P21" s="26"/>
+      <c r="Q21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>45519</v>
       </c>
@@ -1996,10 +2351,13 @@
       <c r="O22" s="6">
         <v>34</v>
       </c>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="P22" s="26"/>
+      <c r="Q22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>45519</v>
       </c>
@@ -2045,10 +2403,13 @@
       <c r="O23" s="6">
         <v>34</v>
       </c>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="P23" s="26"/>
+      <c r="Q23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>45519</v>
       </c>
@@ -2094,10 +2455,11 @@
       <c r="O24" s="6">
         <v>34</v>
       </c>
-      <c r="P24" s="6"/>
+      <c r="P24" s="26"/>
       <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>45519</v>
       </c>
@@ -2143,10 +2505,11 @@
       <c r="O25" s="6">
         <v>34</v>
       </c>
-      <c r="P25" s="6"/>
+      <c r="P25" s="26"/>
       <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>45519</v>
       </c>
@@ -2194,8 +2557,9 @@
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>45519</v>
       </c>
@@ -2243,10 +2607,11 @@
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="R27" s="6"/>
+    </row>
+    <row r="28" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>45519</v>
       </c>
@@ -2269,7 +2634,7 @@
         <v>16</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I28" s="4">
         <v>0.1</v>
@@ -2294,8 +2659,9 @@
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R28" s="6"/>
+    </row>
+    <row r="29" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>45519</v>
       </c>
@@ -2318,7 +2684,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I29" s="4">
         <v>0.01</v>
@@ -2343,8 +2709,9 @@
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
-    </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R29" s="6"/>
+    </row>
+    <row r="30" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>45519</v>
       </c>
@@ -2367,7 +2734,7 @@
         <v>16</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I30" s="4">
         <v>1E-3</v>
@@ -2392,8 +2759,9 @@
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
-    </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R30" s="6"/>
+    </row>
+    <row r="31" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>45519</v>
       </c>
@@ -2416,7 +2784,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I31" s="4">
         <v>1E-4</v>
@@ -2441,8 +2809,9 @@
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
-    </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>45519</v>
       </c>
@@ -2490,8 +2859,9 @@
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
-    </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>45519</v>
       </c>
@@ -2539,8 +2909,9 @@
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
-    </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R33" s="6"/>
+    </row>
+    <row r="34" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>45519</v>
       </c>
@@ -2588,8 +2959,9 @@
       </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R34" s="6"/>
+    </row>
+    <row r="35" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>45519</v>
       </c>
@@ -2637,8 +3009,9 @@
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
-    </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R35" s="6"/>
+    </row>
+    <row r="36" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>45519</v>
       </c>
@@ -2686,8 +3059,9 @@
       </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
-    </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R36" s="6"/>
+    </row>
+    <row r="37" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>45519</v>
       </c>
@@ -2735,8 +3109,9 @@
       </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
-    </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R37" s="6"/>
+    </row>
+    <row r="38" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>45519</v>
       </c>
@@ -2784,8 +3159,9 @@
       </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R38" s="6"/>
+    </row>
+    <row r="39" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>45519</v>
       </c>
@@ -2833,8 +3209,9 @@
       </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
-    </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R39" s="6"/>
+    </row>
+    <row r="40" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>45519</v>
       </c>
@@ -2857,7 +3234,7 @@
         <v>32</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I40" s="4">
         <v>0.1</v>
@@ -2882,8 +3259,9 @@
       </c>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
-    </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R40" s="6"/>
+    </row>
+    <row r="41" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>45519</v>
       </c>
@@ -2906,7 +3284,7 @@
         <v>32</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I41" s="4">
         <v>0.01</v>
@@ -2931,8 +3309,9 @@
       </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
-    </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R41" s="6"/>
+    </row>
+    <row r="42" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45519</v>
       </c>
@@ -2955,7 +3334,7 @@
         <v>32</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I42" s="4">
         <v>1E-3</v>
@@ -2980,8 +3359,9 @@
       </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
-    </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R42" s="6"/>
+    </row>
+    <row r="43" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>45519</v>
       </c>
@@ -3004,7 +3384,7 @@
         <v>32</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I43" s="4">
         <v>1E-4</v>
@@ -3029,8 +3409,9 @@
       </c>
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
-    </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R43" s="6"/>
+    </row>
+    <row r="44" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>45519</v>
       </c>
@@ -3078,8 +3459,9 @@
       </c>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
-    </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R44" s="6"/>
+    </row>
+    <row r="45" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>45519</v>
       </c>
@@ -3127,8 +3509,9 @@
       </c>
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
-    </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R45" s="6"/>
+    </row>
+    <row r="46" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45519</v>
       </c>
@@ -3176,8 +3559,9 @@
       </c>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
-    </row>
-    <row r="47" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R46" s="6"/>
+    </row>
+    <row r="47" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>45519</v>
       </c>
@@ -3225,8 +3609,9 @@
       </c>
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
-    </row>
-    <row r="48" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R47" s="6"/>
+    </row>
+    <row r="48" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>45519</v>
       </c>
@@ -3274,8 +3659,9 @@
       </c>
       <c r="P48" s="6"/>
       <c r="Q48" s="6"/>
-    </row>
-    <row r="49" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R48" s="6"/>
+    </row>
+    <row r="49" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>45519</v>
       </c>
@@ -3323,8 +3709,9 @@
       </c>
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>45519</v>
       </c>
@@ -3372,8 +3759,9 @@
       </c>
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
-    </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R50" s="6"/>
+    </row>
+    <row r="51" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>45519</v>
       </c>
@@ -3421,8 +3809,9 @@
       </c>
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
-    </row>
-    <row r="52" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R51" s="6"/>
+    </row>
+    <row r="52" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>45519</v>
       </c>
@@ -3445,7 +3834,7 @@
         <v>64</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I52" s="4">
         <v>0.1</v>
@@ -3470,8 +3859,9 @@
       </c>
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
-    </row>
-    <row r="53" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>45519</v>
       </c>
@@ -3494,7 +3884,7 @@
         <v>64</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I53" s="4">
         <v>0.01</v>
@@ -3519,8 +3909,9 @@
       </c>
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
-    </row>
-    <row r="54" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>45519</v>
       </c>
@@ -3543,7 +3934,7 @@
         <v>64</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I54" s="4">
         <v>1E-3</v>
@@ -3568,8 +3959,9 @@
       </c>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
-    </row>
-    <row r="55" spans="1:17" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="R54" s="6"/>
+    </row>
+    <row r="55" spans="1:19" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>45519</v>
       </c>
@@ -3592,7 +3984,7 @@
         <v>64</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I55" s="4">
         <v>1E-4</v>
@@ -3617,10 +4009,753 @@
       </c>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+    </row>
+    <row r="56" spans="1:19" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="22">
+        <v>45523</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="24">
+        <v>0.2271</v>
+      </c>
+      <c r="D56" s="24">
+        <v>0.30359999999999998</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="24">
+        <v>30</v>
+      </c>
+      <c r="G56" s="24">
+        <v>32</v>
+      </c>
+      <c r="H56" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="J56" s="23">
+        <v>0</v>
+      </c>
+      <c r="K56" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="N56" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O56" s="23">
+        <v>32</v>
+      </c>
+      <c r="P56" s="27" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q56" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="R56" s="23"/>
+    </row>
+    <row r="57" spans="1:19" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" s="22">
+        <v>45523</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="24">
+        <v>0.49070000000000003</v>
+      </c>
+      <c r="D57" s="24">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="24">
+        <v>30</v>
+      </c>
+      <c r="G57" s="24">
+        <v>32</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="J57" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="K57" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L57" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M57" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="N57" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O57" s="23">
+        <v>32</v>
+      </c>
+      <c r="P57" s="27"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="23"/>
+    </row>
+    <row r="58" spans="1:19" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="22">
+        <v>45523</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="24">
+        <v>0.64790000000000003</v>
+      </c>
+      <c r="D58" s="24">
+        <v>0.67749999999999999</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="24">
+        <v>30</v>
+      </c>
+      <c r="G58" s="24">
+        <v>32</v>
+      </c>
+      <c r="H58" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I58" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="J58" s="23">
+        <v>0</v>
+      </c>
+      <c r="K58" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L58" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M58" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="N58" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O58" s="23">
+        <v>32</v>
+      </c>
+      <c r="P58" s="27"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="23"/>
+    </row>
+    <row r="59" spans="1:19" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A59" s="22">
+        <v>45523</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="24">
+        <v>0.47560000000000002</v>
+      </c>
+      <c r="D59" s="24">
+        <v>0.52090000000000003</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="24">
+        <v>30</v>
+      </c>
+      <c r="G59" s="24">
+        <v>32</v>
+      </c>
+      <c r="H59" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I59" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="J59" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="K59" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M59" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="N59" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O59" s="23">
+        <v>32</v>
+      </c>
+      <c r="P59" s="27"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="23"/>
+    </row>
+    <row r="60" spans="1:19" s="13" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A60" s="12">
+        <v>45523</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0.87290000000000001</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="13">
+        <v>30</v>
+      </c>
+      <c r="G60" s="13">
+        <v>16</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I60" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="J60" s="15">
+        <v>0</v>
+      </c>
+      <c r="K60" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L60" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M60" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N60" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O60" s="15">
+        <v>36</v>
+      </c>
+      <c r="P60" s="15" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q60" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="R60" s="15"/>
+    </row>
+    <row r="61" spans="1:19" s="13" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="12">
+        <v>45523</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="13">
+        <v>0.36470000000000002</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.41460000000000002</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="13">
+        <v>30</v>
+      </c>
+      <c r="G61" s="13">
+        <v>16</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I61" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="J61" s="15">
+        <v>0</v>
+      </c>
+      <c r="K61" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M61" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N61" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O61" s="15">
+        <v>85</v>
+      </c>
+      <c r="P61" s="15" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+    </row>
+    <row r="62" spans="1:19" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="30">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="D62" s="30">
+        <v>0.8206</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="30">
+        <v>60</v>
+      </c>
+      <c r="G62" s="30">
+        <v>16</v>
+      </c>
+      <c r="H62" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I62" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J62" s="29">
+        <v>0</v>
+      </c>
+      <c r="K62" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M62" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N62" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O62" s="29">
+        <v>38</v>
+      </c>
+      <c r="P62" s="31" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q62" s="29" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R62" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A63" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="30">
+        <v>0.97240000000000004</v>
+      </c>
+      <c r="D63" s="30">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="30">
+        <v>60</v>
+      </c>
+      <c r="G63" s="30">
+        <v>16</v>
+      </c>
+      <c r="H63" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I63" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J63" s="29">
+        <v>0</v>
+      </c>
+      <c r="K63" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M63" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N63" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O63" s="29">
+        <v>38</v>
+      </c>
+      <c r="P63" s="31"/>
+      <c r="Q63" s="29" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R63" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" s="30" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="30">
+        <v>0.93440000000000001</v>
+      </c>
+      <c r="D64" s="30">
+        <v>0.84030000000000005</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="30">
+        <v>60</v>
+      </c>
+      <c r="G64" s="30">
+        <v>16</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I64" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J64" s="29">
+        <v>0</v>
+      </c>
+      <c r="K64" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M64" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N64" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O64" s="29">
+        <v>39</v>
+      </c>
+      <c r="P64" s="31"/>
+      <c r="Q64" s="29" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R64" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="S64" s="30" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65" s="30">
+        <v>0.89090000000000003</v>
+      </c>
+      <c r="D65" s="30">
+        <v>0.84819999999999995</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="30">
+        <v>60</v>
+      </c>
+      <c r="G65" s="30">
+        <v>16</v>
+      </c>
+      <c r="H65" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I65" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J65" s="29">
+        <v>0</v>
+      </c>
+      <c r="K65" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M65" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N65" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O65" s="29">
+        <v>39</v>
+      </c>
+      <c r="P65" s="31"/>
+      <c r="Q65" s="29" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R65" s="29"/>
+    </row>
+    <row r="66" spans="1:18" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="30">
+        <v>0.51270000000000004</v>
+      </c>
+      <c r="D66" s="30">
+        <v>0.48930000000000001</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="30">
+        <v>60</v>
+      </c>
+      <c r="G66" s="30">
+        <v>16</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I66" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J66" s="29">
+        <v>0</v>
+      </c>
+      <c r="K66" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M66" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N66" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O66" s="29">
+        <v>34</v>
+      </c>
+      <c r="P66" s="31"/>
+      <c r="Q66" s="29" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R66" s="29"/>
+    </row>
+    <row r="67" spans="1:18" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A67" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="30">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="D67" s="30">
+        <v>0.78259999999999996</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="30">
+        <v>60</v>
+      </c>
+      <c r="G67" s="30">
+        <v>16</v>
+      </c>
+      <c r="H67" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I67" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J67" s="29">
+        <v>0</v>
+      </c>
+      <c r="K67" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M67" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N67" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O67" s="29">
+        <v>35</v>
+      </c>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="29" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R67" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="30">
+        <v>0.63919999999999999</v>
+      </c>
+      <c r="D68" s="30">
+        <v>0.69089999999999996</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="30">
+        <v>60</v>
+      </c>
+      <c r="G68" s="30">
+        <v>16</v>
+      </c>
+      <c r="H68" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I68" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J68" s="29">
+        <v>0</v>
+      </c>
+      <c r="K68" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L68" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M68" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N68" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O68" s="29">
+        <v>35</v>
+      </c>
+      <c r="P68" s="31"/>
+      <c r="Q68" s="29" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R68" s="29"/>
+    </row>
+    <row r="69" spans="1:18" s="30" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="28">
+        <v>45524</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="30">
+        <v>0.71509999999999996</v>
+      </c>
+      <c r="D69" s="30">
+        <v>0.7581</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F69" s="30">
+        <v>60</v>
+      </c>
+      <c r="G69" s="30">
+        <v>16</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="J69" s="29">
+        <v>0</v>
+      </c>
+      <c r="K69" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M69" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="N69" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O69" s="29">
+        <v>36</v>
+      </c>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="29" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R69" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="P13:P15"/>
+    <mergeCell ref="P20:P25"/>
+    <mergeCell ref="P56:P59"/>
+    <mergeCell ref="P62:P68"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>